<commit_message>
Idk wat verandert is
</commit_message>
<xml_diff>
--- a/DistanceMatrix.xlsx
+++ b/DistanceMatrix.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="5" documentId="11_085D87871755860E623554765806C67AADBB842B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76CC36CC-3128-4659-B27C-4912A56D0659}"/>
   <bookViews>
-    <workbookView xWindow="4164" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -123,6 +123,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>